<commit_message>
Migration finished, working on file output
</commit_message>
<xml_diff>
--- a/Drive Teams.xlsx
+++ b/Drive Teams.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2802DF6A-DFD5-4D3C-B545-34D091C2C91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C6B50C-B5B4-4A50-88CE-EA5846C4DCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
   <sheets>
     <sheet name="Match Data" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Data" sheetId="3" r:id="rId3"/>
+    <sheet name="Per Member Data" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1604,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E71918B-9D42-46BC-B578-CF08432FB725}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:H20"/>
+    <sheetView zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3038,4 +3039,16 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F9A13F-868B-4E21-BD8D-3F7EE32D398B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Full implementation and statistics works. Next step is creating a window system
</commit_message>
<xml_diff>
--- a/Drive Teams.xlsx
+++ b/Drive Teams.xlsx
@@ -3,24 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C6B50C-B5B4-4A50-88CE-EA5846C4DCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA45923-966D-47BB-9F22-19B07E715558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
   <sheets>
     <sheet name="Match Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Data" sheetId="3" r:id="rId3"/>
-    <sheet name="Per Member Data" sheetId="4" r:id="rId4"/>
+    <sheet name="Data" sheetId="3" r:id="rId2"/>
+    <sheet name="Per Member Data" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="52">
   <si>
     <t>Cyrus</t>
   </si>
@@ -138,12 +137,70 @@
   </si>
   <si>
     <t>Driver Penalties</t>
+  </si>
+  <si>
+    <t>avgtotal</t>
+  </si>
+  <si>
+    <t>avgtele</t>
+  </si>
+  <si>
+    <t>avgauto</t>
+  </si>
+  <si>
+    <t>avgpen</t>
+  </si>
+  <si>
+    <t>Wavgtele</t>
+  </si>
+  <si>
+    <t>Wavgauto</t>
+  </si>
+  <si>
+    <t>Wavgpen</t>
+  </si>
+  <si>
+    <t>Wavgtot</t>
+  </si>
+  <si>
+    <t>bredan</t>
+  </si>
+  <si>
+    <t>erin</t>
+  </si>
+  <si>
+    <t>luca</t>
+  </si>
+  <si>
+    <t>mason</t>
+  </si>
+  <si>
+    <t>zoe</t>
+  </si>
+  <si>
+    <t>cyrus</t>
+  </si>
+  <si>
+    <t>caleb</t>
+  </si>
+  <si>
+    <t>matt</t>
+  </si>
+  <si>
+    <t>zach</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>**</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -161,12 +218,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -190,12 +253,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1606,13 +1670,13 @@
   <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="10.0"/>
+    <col min="5" max="5" customWidth="true" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -1645,23 +1709,26 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B2" s="1">
         <v>45237</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>106</v>
+      </c>
+      <c r="I2" s="0">
+        <v>0</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1673,443 +1740,681 @@
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B3" s="1">
         <v>45237</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>83</v>
       </c>
+      <c r="I3" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B4" s="1">
         <v>45237</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>89</v>
       </c>
+      <c r="I4" s="0">
+        <v>0</v>
+      </c>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>45238</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>71</v>
       </c>
+      <c r="I5" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B6" s="1">
         <v>45238</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>88</v>
       </c>
+      <c r="I6" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B7" s="1">
         <v>45238</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0">
         <v>111</v>
       </c>
+      <c r="I7" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B8" s="1">
         <v>45238</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0">
         <v>34</v>
       </c>
+      <c r="I8" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>45238</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="0">
         <v>120</v>
       </c>
+      <c r="I9" s="0">
+        <v>0</v>
+      </c>
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B10" s="1">
         <v>45238</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="0">
         <v>75</v>
       </c>
+      <c r="I10" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>45237</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="0">
         <v>111</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="0">
         <v>66</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="0">
         <v>45</v>
       </c>
+      <c r="I11" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>45238</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="0">
         <v>107</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="0">
         <v>57</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="0">
         <v>50</v>
+      </c>
+      <c r="I12" s="0">
+        <v>0</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B13" s="1">
         <v>45234</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="0">
         <v>72</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="0">
         <v>44</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="0">
         <v>28</v>
       </c>
+      <c r="I13" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B14" s="1">
         <v>45234</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="0">
         <v>97</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="0">
         <v>51</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="0">
         <v>30</v>
       </c>
+      <c r="I14" s="0">
+        <v>0</v>
+      </c>
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B15" s="1">
         <v>45234</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="0">
         <v>54</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="0">
         <v>26</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="0">
         <v>28</v>
       </c>
+      <c r="I15" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B16" s="1">
         <v>45234</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="0">
         <v>82</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="0">
         <v>32</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="0">
         <v>50</v>
       </c>
+      <c r="I16" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B17" s="1">
         <v>45234</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="0">
         <v>60</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="0">
         <v>40</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="0">
         <v>20</v>
       </c>
+      <c r="I17" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>45234</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="0">
         <v>56</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="0">
         <v>48</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="0">
         <v>8</v>
       </c>
+      <c r="I18" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B19" s="1">
         <v>45234</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="0">
         <v>60</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="0">
         <v>30</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="0">
         <v>30</v>
       </c>
+      <c r="I19" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B20" s="1">
         <v>45234</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="0">
         <v>39</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="0">
         <v>34</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="0">
         <v>5</v>
       </c>
+      <c r="I20" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A21" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45241</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0">
+        <v>32</v>
+      </c>
+      <c r="G21" s="0">
+        <v>4</v>
+      </c>
+      <c r="H21" s="0">
+        <v>28</v>
+      </c>
+      <c r="I21" s="0">
+        <v>0</v>
+      </c>
+      <c r="K21" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A22" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45241</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="F22" s="0">
+        <v>83</v>
+      </c>
+      <c r="G22" s="0">
+        <v>55</v>
+      </c>
+      <c r="H22" s="0">
+        <v>28</v>
+      </c>
+      <c r="I22" s="0">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A23" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45241</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="F23" s="0">
+        <v>56</v>
+      </c>
+      <c r="G23" s="0">
+        <v>26</v>
+      </c>
+      <c r="H23" s="0">
+        <v>30</v>
+      </c>
+      <c r="I23" s="0">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A24" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B24" s="1">
+        <v>45241</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="F24" s="0">
+        <v>33</v>
+      </c>
+      <c r="G24" s="0">
+        <v>28</v>
+      </c>
+      <c r="H24" s="0">
+        <v>5</v>
+      </c>
+      <c r="I24" s="0">
+        <v>0</v>
+      </c>
+      <c r="K24" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A25" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45241</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="F25" s="0">
+        <v>56</v>
+      </c>
+      <c r="G25" s="0">
+        <v>36</v>
+      </c>
+      <c r="H25" s="0">
+        <v>20</v>
+      </c>
+      <c r="I25" s="0">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s" s="0">
+        <v>50</v>
+      </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T26" s="5"/>
-      <c r="U26" s="5"/>
-      <c r="V26" s="5"/>
-      <c r="W26" s="5"/>
+      <c r="A26" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45241</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="I26" s="0">
+        <v>0</v>
+      </c>
+      <c r="J26" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="K26" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="6"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T31" s="5"/>
-      <c r="U31" s="5"/>
-      <c r="V31" s="5"/>
-      <c r="W31" s="5"/>
+      <c r="T31" s="6"/>
+      <c r="U31" s="6"/>
+      <c r="V31" s="6"/>
+      <c r="W31" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2122,20 +2427,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30E5E941-ADA4-4E7B-8BA3-E27502D0AB4A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0F5FA5-EAA3-4AD1-96C5-3162EEB9C9CF}">
   <dimension ref="A2:Y35"/>
   <sheetViews>
@@ -2145,8 +2436,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="10.0"/>
+    <col min="5" max="5" customWidth="true" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -2178,7 +2469,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="V2" t="s">
+      <c r="V2" t="s" s="0">
         <v>18</v>
       </c>
     </row>
@@ -2186,16 +2477,16 @@
       <c r="A3" s="1">
         <v>45237</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <v>106</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>1</v>
       </c>
     </row>
@@ -2203,25 +2494,25 @@
       <c r="A4" s="1">
         <v>45237</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0">
         <v>83</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" t="s" s="0">
         <v>24</v>
       </c>
     </row>
@@ -2229,26 +2520,26 @@
       <c r="A5" s="1">
         <v>45237</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0">
         <v>89</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="0">
         <f>(SUMIF($C$3:$C$100, M5, $B$3:$B$100)/COUNTIF($C$3:$C$100, M5))</f>
         <v>88.083333333333329</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="0">
         <f>(SUMIF($C$3:$C$100, M5, $F$3:$F$100)/COUNTIF($C$13:$C$100, M5))</f>
         <v>42.428571428571431</v>
       </c>
@@ -2257,26 +2548,26 @@
       <c r="A6" s="1">
         <v>45238</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="0">
         <v>71</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="0">
         <f>(SUMIF($C$3:$C$100, M6, $B$3:$B$100)/COUNTIF($C$3:$C$100, M6))</f>
         <v>98.5</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="0">
         <f>(SUMIF($C$3:$C$100, M6, $F$3:$F$100)/COUNTIF($C$13:$C$100, M6))</f>
         <v>57.333333333333336</v>
       </c>
@@ -2285,26 +2576,26 @@
       <c r="A7" s="1">
         <v>45238</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="0">
         <v>88</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="0">
         <f>(SUMIF($C$3:$C$100, M7, $B$3:$B$100)/COUNTIF($C$3:$C$100, M7))</f>
         <v>86.25</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="0">
         <f>(SUMIF($C$3:$C$100, M7, $F$3:$F$100)/COUNTIF($C$13:$C$100, M7))</f>
         <v>38</v>
       </c>
@@ -2313,16 +2604,16 @@
       <c r="A8" s="1">
         <v>45238</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="0">
         <v>111</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>1</v>
       </c>
     </row>
@@ -2330,16 +2621,16 @@
       <c r="A9" s="1">
         <v>45238</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="0">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>1</v>
       </c>
       <c r="M9" s="2" t="s">
@@ -2350,32 +2641,32 @@
       <c r="A10" s="1">
         <v>45238</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="0">
         <v>120</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="M10" t="s">
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="M10" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="0">
         <f>(SUMIF($D$3:$D$100, M10, $B$3:$B$100)/COUNTIF($D$3:$D$100, M10))</f>
         <v>96.666666666666671</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="0">
         <f>(SUMIF($D$3:$D$100, M10, $F$3:$F$100)/COUNTIF($D$13:$D$100, M10))</f>
         <v>26</v>
       </c>
@@ -2384,34 +2675,34 @@
       <c r="A11" s="1">
         <v>45238</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="0">
         <v>75</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="6" t="s">
+      <c r="I11" s="6"/>
+      <c r="J11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="5"/>
-      <c r="M11" t="s">
+      <c r="K11" s="6"/>
+      <c r="M11" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="0">
         <f>(SUMIF($D$3:$D$100, M11, $B$3:$B$100)/COUNTIF($D$3:$D$100, M11))</f>
         <v>77</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="0">
         <f>(SUMIF($D$3:$D$100, M11, $F$3:$F$100)/COUNTIF($D$13:$D$100, M11))</f>
         <v>45.166666666666664</v>
       </c>
@@ -2429,14 +2720,14 @@
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="0">
         <f>(SUMIF($D$3:$D$100, M12, $B$3:$B$100)/COUNTIF($D$3:$D$100, M12))</f>
         <v>97.75</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="0">
         <f>(SUMIF($D$3:$D$100, M12, $F$3:$F$100)/COUNTIF($D$13:$D$100, M12))</f>
         <v>57.333333333333336</v>
       </c>
@@ -2445,26 +2736,26 @@
       <c r="A13" s="1">
         <v>45237</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="0">
         <v>111</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="0">
         <v>66</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="0">
         <f t="shared" ref="H13:H23" si="0">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12)+SUMIF($M$15:$M$17, $E13, $N$15:$N$17))/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="0">
         <f t="shared" ref="I13:I23" si="1">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12)+SUMIF($M$15:$M$17, $E13, $O$15:$O$17))/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -2472,7 +2763,7 @@
         <f t="shared" ref="J13:J23" si="2">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12))/2</f>
         <v>98.125</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="0">
         <f t="shared" ref="K13:K23" si="3">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12))/2</f>
         <v>57.333333333333336</v>
       </c>
@@ -2481,26 +2772,26 @@
       <c r="A14" s="1">
         <v>45238</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="0">
         <v>107</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="0">
         <v>57</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="0">
         <f t="shared" si="0"/>
         <v>84.49444444444444</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="0">
         <f t="shared" si="1"/>
         <v>48.198412698412703</v>
       </c>
@@ -2508,7 +2799,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -2520,26 +2811,26 @@
       <c r="A15" s="1">
         <v>45234</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="0">
         <v>108</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="0">
         <v>38</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="0">
         <f t="shared" si="0"/>
         <v>63.166666666666664</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="0">
         <f t="shared" si="1"/>
         <v>30.166666666666668</v>
       </c>
@@ -2547,18 +2838,18 @@
         <f t="shared" si="2"/>
         <v>43.125</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="0">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M15" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="0">
         <f>(SUMIF($E$3:$E$100, M15, $B$3:$B$100)/COUNTIF($E$3:$E$100, M15))</f>
         <v>83.166666666666671</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="0">
         <f>(SUMIF($E$3:$E$100, M15, $F$3:$F$100)/COUNTIF($E$13:$E$100, M15))</f>
         <v>40</v>
       </c>
@@ -2567,26 +2858,26 @@
       <c r="A16" s="1">
         <v>45234</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="0">
         <v>107</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="0">
         <v>74</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="0">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="0">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -2594,18 +2885,18 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="0">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="0">
         <f>(SUMIF($E$3:$E$100, M16, $B$3:$B$100)/COUNTIF($E$3:$E$100, M16))</f>
         <v>88.4</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="0">
         <f>(SUMIF($E$3:$E$100, M16, $F$3:$F$100)/COUNTIF($E$13:$E$100, M16))</f>
         <v>57</v>
       </c>
@@ -2614,26 +2905,26 @@
       <c r="A17" s="1">
         <v>45234</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="0">
         <v>97</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="0">
         <v>62</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -2641,18 +2932,18 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="0">
         <f>(SUMIF($E$3:$E$100, M17, $B$3:$B$100)/COUNTIF($E$3:$E$100, M17))</f>
         <v>103.25</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="0">
         <f>(SUMIF($E$3:$E$100, M17, $F$3:$F$100)/COUNTIF($E$13:$E$100, M17))</f>
         <v>52.5</v>
       </c>
@@ -2661,26 +2952,26 @@
       <c r="A18" s="1">
         <v>45234</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="0">
         <v>99</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="0">
         <v>26</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="0">
         <f t="shared" si="0"/>
         <v>89.305555555555557</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="0">
         <f t="shared" si="1"/>
         <v>36.142857142857146</v>
       </c>
@@ -2688,7 +2979,7 @@
         <f t="shared" si="2"/>
         <v>92.375</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="0">
         <f t="shared" si="3"/>
         <v>34.214285714285715</v>
       </c>
@@ -2697,26 +2988,26 @@
       <c r="A19" s="1">
         <v>45234</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="0">
         <v>87</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="0">
         <v>32</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="0">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="0">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -2724,7 +3015,7 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="0">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
@@ -2733,26 +3024,26 @@
       <c r="A20" s="1">
         <v>45234</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="0">
         <v>76</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="0">
         <v>48</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -2760,7 +3051,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -2769,26 +3060,26 @@
       <c r="A21" s="1">
         <v>45234</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="0">
         <v>93</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="0">
         <v>40</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -2796,7 +3087,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -2805,26 +3096,26 @@
       <c r="A22" s="1">
         <v>45234</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="0">
         <v>85</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="0">
         <v>30</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -2832,7 +3123,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -2841,26 +3132,26 @@
       <c r="A23" s="1">
         <v>45234</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="0">
         <v>49</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="0">
         <v>34</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -2868,18 +3159,18 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T27" s="5" t="s">
+      <c r="T27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="U27" s="5"/>
-      <c r="V27" s="5"/>
-      <c r="W27" s="5"/>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
       <c r="X27" s="2" t="s">
         <v>23</v>
       </c>
@@ -2888,141 +3179,141 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T28">
+      <c r="T28" s="0">
         <v>1</v>
       </c>
-      <c r="U28" t="s">
+      <c r="U28" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="V28" t="s">
+      <c r="V28" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="W28" t="s">
+      <c r="W28" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X28">
+      <c r="X28" s="0">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y28">
+      <c r="Y28" s="0">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T29">
+      <c r="T29" s="0">
         <v>2</v>
       </c>
-      <c r="U29" t="s">
+      <c r="U29" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="V29" t="s">
+      <c r="V29" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="W29" t="s">
+      <c r="W29" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X29">
+      <c r="X29" s="0">
         <f>(N5+N11+N16)/3</f>
         <v>84.49444444444444</v>
       </c>
-      <c r="Y29">
+      <c r="Y29" s="0">
         <f>(O5+O11+O16)/3</f>
         <v>48.198412698412703</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T30">
+      <c r="T30" s="0">
         <v>3</v>
       </c>
-      <c r="U30" t="s">
+      <c r="U30" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="V30" t="s">
+      <c r="V30" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="W30" t="s">
+      <c r="W30" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X30">
+      <c r="X30" s="0">
         <f>(N6+N11+N16)/3</f>
         <v>87.966666666666654</v>
       </c>
-      <c r="Y30">
+      <c r="Y30" s="0">
         <f>(O6+O11+O16)/3</f>
         <v>53.166666666666664</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T32" s="5" t="s">
+      <c r="T32" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="U32" s="5"/>
-      <c r="V32" s="5"/>
-      <c r="W32" s="5"/>
+      <c r="U32" s="6"/>
+      <c r="V32" s="6"/>
+      <c r="W32" s="6"/>
     </row>
     <row r="33" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T33">
+      <c r="T33" s="0">
         <v>1</v>
       </c>
-      <c r="U33" t="s">
+      <c r="U33" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="V33" t="s">
+      <c r="V33" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="W33" t="s">
+      <c r="W33" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X33">
+      <c r="X33" s="0">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y33">
+      <c r="Y33" s="0">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="34" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T34">
+      <c r="T34" s="0">
         <v>2</v>
       </c>
-      <c r="U34" t="s">
+      <c r="U34" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="V34" t="s">
+      <c r="V34" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="W34" t="s">
+      <c r="W34" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="X34">
+      <c r="X34" s="0">
         <f>(N5+N11+N15)/3</f>
         <v>82.75</v>
       </c>
-      <c r="Y34">
+      <c r="Y34" s="0">
         <f>(O5+O11+O15)/3</f>
         <v>42.531746031746032</v>
       </c>
     </row>
     <row r="35" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T35">
+      <c r="T35" s="0">
         <v>3</v>
       </c>
-      <c r="U35" t="s">
+      <c r="U35" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="V35" t="s">
+      <c r="V35" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="W35" t="s">
+      <c r="W35" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="X35">
+      <c r="X35" s="0">
         <f>(N6+N12+N17)/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="Y35">
+      <c r="Y35" s="0">
         <f>(O6+O12+O17)/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -3041,14 +3332,304 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F9A13F-868B-4E21-BD8D-3F7EE32D398B}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="n" s="0">
+        <v>70.64285714285714</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>35.333333333333336</v>
+      </c>
+      <c r="C2" t="n" s="0">
+        <v>22.666666666666668</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>70.56385542170489</v>
+      </c>
+      <c r="F2" t="n" s="0">
+        <v>34.62835249058675</v>
+      </c>
+      <c r="G2" t="n" s="0">
+        <v>22.754789272009987</v>
+      </c>
+      <c r="H2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="n" s="0">
+        <v>82.16666666666667</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>46.6</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>34.2</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>81.78021978030641</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>46.881578947305435</v>
+      </c>
+      <c r="G3" t="n" s="0">
+        <v>33.47368421068877</v>
+      </c>
+      <c r="H3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="n" s="0">
+        <v>73.25</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>26.0</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>30.0</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>72.76190476201013</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>26.0</v>
+      </c>
+      <c r="G4" t="n" s="0">
+        <v>30.0</v>
+      </c>
+      <c r="H4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M4" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="n" s="0">
+        <v>61.0</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>38.3</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>22.4</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E5" t="n" s="0">
+        <v>60.59340659349776</v>
+      </c>
+      <c r="F5" t="n" s="0">
+        <v>37.847682119307144</v>
+      </c>
+      <c r="G5" t="n" s="0">
+        <v>22.566225165525484</v>
+      </c>
+      <c r="H5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M5" t="s" s="0">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="n" s="0">
+        <v>92.75</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <v>47.333333333333336</v>
+      </c>
+      <c r="C6" t="n" s="0">
+        <v>41.0</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E6" t="n" s="0">
+        <v>93.20762711853857</v>
+      </c>
+      <c r="F6" t="n" s="0">
+        <v>47.999999999838096</v>
+      </c>
+      <c r="G6" t="n" s="0">
+        <v>41.14285714282244</v>
+      </c>
+      <c r="H6" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M6" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="n" s="0">
+        <v>75.25</v>
+      </c>
+      <c r="B7" t="n" s="0">
+        <v>26.0</v>
+      </c>
+      <c r="C7" t="n" s="0">
+        <v>29.0</v>
+      </c>
+      <c r="D7" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E7" t="n" s="0">
+        <v>75.47154471539817</v>
+      </c>
+      <c r="F7" t="n" s="0">
+        <v>25.999999999999996</v>
+      </c>
+      <c r="G7" t="n" s="0">
+        <v>29.11475409833507</v>
+      </c>
+      <c r="H7" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M7" t="s" s="0">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="n" s="0">
+        <v>61.0</v>
+      </c>
+      <c r="B8" t="n" s="0">
+        <v>38.166666666666664</v>
+      </c>
+      <c r="C8" t="n" s="0">
+        <v>20.166666666666668</v>
+      </c>
+      <c r="D8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E8" t="n" s="0">
+        <v>60.999999999999986</v>
+      </c>
+      <c r="F8" t="n" s="0">
+        <v>38.166666666666664</v>
+      </c>
+      <c r="G8" t="n" s="0">
+        <v>20.166666666666664</v>
+      </c>
+      <c r="H8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M8" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="n" s="0">
+        <v>88.33333333333333</v>
+      </c>
+      <c r="B9" t="n" s="0">
+        <v>47.333333333333336</v>
+      </c>
+      <c r="C9" t="n" s="0">
+        <v>41.0</v>
+      </c>
+      <c r="D9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E9" t="n" s="0">
+        <v>89.14285714266053</v>
+      </c>
+      <c r="F9" t="n" s="0">
+        <v>47.999999999838096</v>
+      </c>
+      <c r="G9" t="n" s="0">
+        <v>41.14285714282244</v>
+      </c>
+      <c r="H9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M9" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="n" s="0">
+        <v>76.26666666666667</v>
+      </c>
+      <c r="B10" t="n" s="0">
+        <v>34.333333333333336</v>
+      </c>
+      <c r="C10" t="n" s="0">
+        <v>26.833333333333332</v>
+      </c>
+      <c r="D10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E10" t="n" s="0">
+        <v>75.40041928739694</v>
+      </c>
+      <c r="F10" t="n" s="0">
+        <v>33.99502487569056</v>
+      </c>
+      <c r="G10" t="n" s="0">
+        <v>26.487562189124915</v>
+      </c>
+      <c r="H10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M10" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
It's ugly but it works
</commit_message>
<xml_diff>
--- a/Drive Teams.xlsx
+++ b/Drive Teams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA45923-966D-47BB-9F22-19B07E715558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D388E83-6827-4654-9F37-824FD332ED45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
+    <workbookView xWindow="3792" yWindow="2400" windowWidth="17280" windowHeight="8880" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
   <sheets>
     <sheet name="Match Data" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="52">
   <si>
     <t>Cyrus</t>
   </si>
@@ -193,7 +193,7 @@
     <t>*</t>
   </si>
   <si>
-    <t>**</t>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -218,18 +218,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -253,13 +247,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1667,10 +1660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E71918B-9D42-46BC-B578-CF08432FB725}">
-  <dimension ref="A1:Y31"/>
+  <dimension ref="A1:Y33"/>
   <sheetViews>
-    <sheetView zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I29" sqref="A27:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2257,10 +2250,10 @@
       <c r="B22" s="1">
         <v>45241</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" t="s" s="0">
         <v>9</v>
       </c>
       <c r="E22" t="s" s="0">
@@ -2289,10 +2282,10 @@
       <c r="B23" s="1">
         <v>45241</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" t="s" s="0">
         <v>0</v>
       </c>
       <c r="E23" t="s" s="0">
@@ -2321,10 +2314,10 @@
       <c r="B24" s="1">
         <v>45241</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" t="s" s="0">
         <v>9</v>
       </c>
       <c r="E24" t="s" s="0">
@@ -2353,7 +2346,7 @@
       <c r="B25" s="1">
         <v>45241</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" t="s" s="0">
         <v>4</v>
       </c>
       <c r="D25" t="s" s="0">
@@ -2385,36 +2378,103 @@
       <c r="B26" s="1">
         <v>45241</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" t="s" s="0">
         <v>0</v>
       </c>
       <c r="E26" t="s" s="0">
         <v>1</v>
       </c>
+      <c r="F26" s="0">
+        <v>55</v>
+      </c>
+      <c r="G26" s="0">
+        <v>27</v>
+      </c>
+      <c r="H26" s="0">
+        <v>28</v>
+      </c>
       <c r="I26" s="0">
         <v>0</v>
-      </c>
-      <c r="J26" t="s" s="0">
-        <v>51</v>
       </c>
       <c r="K26" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
-      <c r="V26" s="6"/>
-      <c r="W26" s="6"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
     </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B27" s="0"/>
+      <c r="C27" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="F27" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="G27" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="H27" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="I27" t="n" s="0">
+        <v>10.0</v>
+      </c>
+    </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T31" s="6"/>
-      <c r="U31" s="6"/>
-      <c r="V31" s="6"/>
-      <c r="W31" s="6"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="5"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A32" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="F32" s="0">
+        <v>10</v>
+      </c>
+      <c r="G32" s="0">
+        <v>10</v>
+      </c>
+      <c r="H32" s="0">
+        <v>56</v>
+      </c>
+      <c r="I32" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="F33" s="0">
+        <v>10</v>
+      </c>
+      <c r="G33" s="0">
+        <v>10</v>
+      </c>
+      <c r="H33" s="0">
+        <v>56</v>
+      </c>
+      <c r="I33" s="0">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2653,12 +2713,12 @@
       <c r="E10" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
       <c r="M10" t="s" s="0">
         <v>0</v>
       </c>
@@ -2687,14 +2747,14 @@
       <c r="E11" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="7" t="s">
+      <c r="I11" s="5"/>
+      <c r="J11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="6"/>
+      <c r="K11" s="5"/>
       <c r="M11" t="s" s="0">
         <v>9</v>
       </c>
@@ -3165,12 +3225,12 @@
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T27" s="6" t="s">
+      <c r="T27" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="U27" s="6"/>
-      <c r="V27" s="6"/>
-      <c r="W27" s="6"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
       <c r="X27" s="2" t="s">
         <v>23</v>
       </c>
@@ -3245,12 +3305,12 @@
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T32" s="6" t="s">
+      <c r="T32" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="U32" s="6"/>
-      <c r="V32" s="6"/>
-      <c r="W32" s="6"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
     </row>
     <row r="33" spans="20:25" x14ac:dyDescent="0.3">
       <c r="T33" s="0">
@@ -3336,7 +3396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
@@ -3369,261 +3429,261 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="n" s="0">
-        <v>70.64285714285714</v>
-      </c>
-      <c r="B2" t="n" s="0">
+      <c r="A2" s="0">
+        <v>70.642857142857139</v>
+      </c>
+      <c r="B2" s="0">
         <v>35.333333333333336</v>
       </c>
-      <c r="C2" t="n" s="0">
+      <c r="C2" s="0">
         <v>22.666666666666668</v>
       </c>
-      <c r="D2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E2" t="n" s="0">
-        <v>70.56385542170489</v>
-      </c>
-      <c r="F2" t="n" s="0">
-        <v>34.62835249058675</v>
-      </c>
-      <c r="G2" t="n" s="0">
+      <c r="D2" s="0">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0">
+        <v>70.563855421704886</v>
+      </c>
+      <c r="F2" s="0">
+        <v>34.628352490586749</v>
+      </c>
+      <c r="G2" s="0">
         <v>22.754789272009987</v>
       </c>
-      <c r="H2" t="n" s="0">
-        <v>0.0</v>
+      <c r="H2" s="0">
+        <v>0</v>
       </c>
       <c r="M2" t="s" s="0">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="n" s="0">
-        <v>82.16666666666667</v>
-      </c>
-      <c r="B3" t="n" s="0">
+      <c r="A3" s="0">
+        <v>82.166666666666671</v>
+      </c>
+      <c r="B3" s="0">
         <v>46.6</v>
       </c>
-      <c r="C3" t="n" s="0">
-        <v>34.2</v>
-      </c>
-      <c r="D3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E3" t="n" s="0">
+      <c r="C3" s="0">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="D3" s="0">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0">
         <v>81.78021978030641</v>
       </c>
-      <c r="F3" t="n" s="0">
+      <c r="F3" s="0">
         <v>46.881578947305435</v>
       </c>
-      <c r="G3" t="n" s="0">
-        <v>33.47368421068877</v>
-      </c>
-      <c r="H3" t="n" s="0">
-        <v>0.0</v>
+      <c r="G3" s="0">
+        <v>33.473684210688774</v>
+      </c>
+      <c r="H3" s="0">
+        <v>0</v>
       </c>
       <c r="M3" t="s" s="0">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="n" s="0">
+      <c r="A4" s="0">
         <v>73.25</v>
       </c>
-      <c r="B4" t="n" s="0">
-        <v>26.0</v>
-      </c>
-      <c r="C4" t="n" s="0">
-        <v>30.0</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E4" t="n" s="0">
-        <v>72.76190476201013</v>
-      </c>
-      <c r="F4" t="n" s="0">
-        <v>26.0</v>
-      </c>
-      <c r="G4" t="n" s="0">
-        <v>30.0</v>
-      </c>
-      <c r="H4" t="n" s="0">
-        <v>0.0</v>
+      <c r="B4" s="0">
+        <v>26</v>
+      </c>
+      <c r="C4" s="0">
+        <v>30</v>
+      </c>
+      <c r="D4" s="0">
+        <v>0</v>
+      </c>
+      <c r="E4" s="0">
+        <v>72.761904762010133</v>
+      </c>
+      <c r="F4" s="0">
+        <v>26</v>
+      </c>
+      <c r="G4" s="0">
+        <v>30</v>
+      </c>
+      <c r="H4" s="0">
+        <v>0</v>
       </c>
       <c r="M4" t="s" s="0">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="n" s="0">
-        <v>61.0</v>
-      </c>
-      <c r="B5" t="n" s="0">
-        <v>38.3</v>
-      </c>
-      <c r="C5" t="n" s="0">
+      <c r="A5" s="0">
+        <v>61</v>
+      </c>
+      <c r="B5" s="0">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="C5" s="0">
         <v>22.4</v>
       </c>
-      <c r="D5" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E5" t="n" s="0">
-        <v>60.59340659349776</v>
-      </c>
-      <c r="F5" t="n" s="0">
+      <c r="D5" s="0">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0">
+        <v>60.593406593497761</v>
+      </c>
+      <c r="F5" s="0">
         <v>37.847682119307144</v>
       </c>
-      <c r="G5" t="n" s="0">
+      <c r="G5" s="0">
         <v>22.566225165525484</v>
       </c>
-      <c r="H5" t="n" s="0">
-        <v>0.0</v>
+      <c r="H5" s="0">
+        <v>0</v>
       </c>
       <c r="M5" t="s" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="n" s="0">
+      <c r="A6" s="0">
         <v>92.75</v>
       </c>
-      <c r="B6" t="n" s="0">
+      <c r="B6" s="0">
         <v>47.333333333333336</v>
       </c>
-      <c r="C6" t="n" s="0">
-        <v>41.0</v>
-      </c>
-      <c r="D6" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E6" t="n" s="0">
-        <v>93.20762711853857</v>
-      </c>
-      <c r="F6" t="n" s="0">
+      <c r="C6" s="0">
+        <v>41</v>
+      </c>
+      <c r="D6" s="0">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0">
+        <v>93.207627118538568</v>
+      </c>
+      <c r="F6" s="0">
         <v>47.999999999838096</v>
       </c>
-      <c r="G6" t="n" s="0">
-        <v>41.14285714282244</v>
-      </c>
-      <c r="H6" t="n" s="0">
-        <v>0.0</v>
+      <c r="G6" s="0">
+        <v>41.142857142822443</v>
+      </c>
+      <c r="H6" s="0">
+        <v>0</v>
       </c>
       <c r="M6" t="s" s="0">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="n" s="0">
+      <c r="A7" s="0">
         <v>75.25</v>
       </c>
-      <c r="B7" t="n" s="0">
-        <v>26.0</v>
-      </c>
-      <c r="C7" t="n" s="0">
-        <v>29.0</v>
-      </c>
-      <c r="D7" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E7" t="n" s="0">
-        <v>75.47154471539817</v>
-      </c>
-      <c r="F7" t="n" s="0">
+      <c r="B7" s="0">
+        <v>26</v>
+      </c>
+      <c r="C7" s="0">
+        <v>29</v>
+      </c>
+      <c r="D7" s="0">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0">
+        <v>75.471544715398167</v>
+      </c>
+      <c r="F7" s="0">
         <v>25.999999999999996</v>
       </c>
-      <c r="G7" t="n" s="0">
-        <v>29.11475409833507</v>
-      </c>
-      <c r="H7" t="n" s="0">
-        <v>0.0</v>
+      <c r="G7" s="0">
+        <v>29.114754098335069</v>
+      </c>
+      <c r="H7" s="0">
+        <v>0</v>
       </c>
       <c r="M7" t="s" s="0">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="n" s="0">
-        <v>61.0</v>
-      </c>
-      <c r="B8" t="n" s="0">
+      <c r="A8" s="0">
+        <v>61</v>
+      </c>
+      <c r="B8" s="0">
         <v>38.166666666666664</v>
       </c>
-      <c r="C8" t="n" s="0">
+      <c r="C8" s="0">
         <v>20.166666666666668</v>
       </c>
-      <c r="D8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E8" t="n" s="0">
+      <c r="D8" s="0">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0">
         <v>60.999999999999986</v>
       </c>
-      <c r="F8" t="n" s="0">
+      <c r="F8" s="0">
         <v>38.166666666666664</v>
       </c>
-      <c r="G8" t="n" s="0">
+      <c r="G8" s="0">
         <v>20.166666666666664</v>
       </c>
-      <c r="H8" t="n" s="0">
-        <v>0.0</v>
+      <c r="H8" s="0">
+        <v>0</v>
       </c>
       <c r="M8" t="s" s="0">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" t="n" s="0">
-        <v>88.33333333333333</v>
-      </c>
-      <c r="B9" t="n" s="0">
+      <c r="A9" s="0">
+        <v>88.333333333333329</v>
+      </c>
+      <c r="B9" s="0">
         <v>47.333333333333336</v>
       </c>
-      <c r="C9" t="n" s="0">
-        <v>41.0</v>
-      </c>
-      <c r="D9" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E9" t="n" s="0">
-        <v>89.14285714266053</v>
-      </c>
-      <c r="F9" t="n" s="0">
+      <c r="C9" s="0">
+        <v>41</v>
+      </c>
+      <c r="D9" s="0">
+        <v>0</v>
+      </c>
+      <c r="E9" s="0">
+        <v>89.142857142660532</v>
+      </c>
+      <c r="F9" s="0">
         <v>47.999999999838096</v>
       </c>
-      <c r="G9" t="n" s="0">
-        <v>41.14285714282244</v>
-      </c>
-      <c r="H9" t="n" s="0">
-        <v>0.0</v>
+      <c r="G9" s="0">
+        <v>41.142857142822443</v>
+      </c>
+      <c r="H9" s="0">
+        <v>0</v>
       </c>
       <c r="M9" t="s" s="0">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" t="n" s="0">
-        <v>76.26666666666667</v>
-      </c>
-      <c r="B10" t="n" s="0">
+      <c r="A10" s="0">
+        <v>76.266666666666666</v>
+      </c>
+      <c r="B10" s="0">
         <v>34.333333333333336</v>
       </c>
-      <c r="C10" t="n" s="0">
+      <c r="C10" s="0">
         <v>26.833333333333332</v>
       </c>
-      <c r="D10" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E10" t="n" s="0">
-        <v>75.40041928739694</v>
-      </c>
-      <c r="F10" t="n" s="0">
-        <v>33.99502487569056</v>
-      </c>
-      <c r="G10" t="n" s="0">
+      <c r="D10" s="0">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0">
+        <v>75.400419287396943</v>
+      </c>
+      <c r="F10" s="0">
+        <v>33.995024875690561</v>
+      </c>
+      <c r="G10" s="0">
         <v>26.487562189124915</v>
       </c>
-      <c r="H10" t="n" s="0">
-        <v>0.0</v>
+      <c r="H10" s="0">
+        <v>0</v>
       </c>
       <c r="M10" t="s" s="0">
         <v>49</v>

</xml_diff>

<commit_message>
Entry fields and buttons now scale with screen size
</commit_message>
<xml_diff>
--- a/Drive Teams.xlsx
+++ b/Drive Teams.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D388E83-6827-4654-9F37-824FD332ED45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A2227F-1C3A-4C6F-A395-EEE5D6D3CBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3792" yWindow="2400" windowWidth="17280" windowHeight="8880" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="52">
   <si>
     <t>Cyrus</t>
   </si>
@@ -200,7 +200,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1663,13 +1662,13 @@
   <dimension ref="A1:Y33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I29" sqref="A27:I29"/>
+      <selection activeCell="I27" sqref="A27:I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="10.0"/>
-    <col min="5" max="5" customWidth="true" width="10.6640625"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -1702,25 +1701,25 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1">
         <v>45237</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2">
         <v>106</v>
       </c>
-      <c r="I2" s="0">
+      <c r="I2">
         <v>0</v>
       </c>
       <c r="M2" s="2"/>
@@ -1733,673 +1732,673 @@
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="1">
         <v>45237</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3">
         <v>83</v>
       </c>
-      <c r="I3" s="0">
+      <c r="I3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="1">
         <v>45237</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F4">
         <v>89</v>
       </c>
-      <c r="I4" s="0">
+      <c r="I4">
         <v>0</v>
       </c>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>45238</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s" s="0">
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="0">
+      <c r="F5">
         <v>71</v>
       </c>
-      <c r="I5" s="0">
+      <c r="I5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="1">
         <v>45238</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="0">
+      <c r="F6">
         <v>88</v>
       </c>
-      <c r="I6" s="0">
+      <c r="I6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="1">
         <v>45238</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s" s="0">
+      <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="0">
+      <c r="F7">
         <v>111</v>
       </c>
-      <c r="I7" s="0">
+      <c r="I7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="1">
         <v>45238</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="E8" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="0">
+      <c r="F8">
         <v>34</v>
       </c>
-      <c r="I8" s="0">
+      <c r="I8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>45238</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s" s="0">
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="0">
+      <c r="F9">
         <v>120</v>
       </c>
-      <c r="I9" s="0">
+      <c r="I9">
         <v>0</v>
       </c>
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1">
         <v>45238</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s" s="0">
+      <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s" s="0">
+      <c r="E10" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="0">
+      <c r="F10">
         <v>75</v>
       </c>
-      <c r="I10" s="0">
+      <c r="I10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" t="s" s="0">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>45237</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>2</v>
       </c>
-      <c r="E11" t="s" s="0">
+      <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="0">
+      <c r="F11">
         <v>111</v>
       </c>
-      <c r="G11" s="0">
+      <c r="G11">
         <v>66</v>
       </c>
-      <c r="H11" s="0">
+      <c r="H11">
         <v>45</v>
       </c>
-      <c r="I11" s="0">
+      <c r="I11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" t="s" s="0">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>45238</v>
       </c>
-      <c r="C12" t="s" s="0">
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="s" s="0">
+      <c r="D12" t="s">
         <v>9</v>
       </c>
-      <c r="E12" t="s" s="0">
+      <c r="E12" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="0">
+      <c r="F12">
         <v>107</v>
       </c>
-      <c r="G12" s="0">
+      <c r="G12">
         <v>57</v>
       </c>
-      <c r="H12" s="0">
+      <c r="H12">
         <v>50</v>
       </c>
-      <c r="I12" s="0">
+      <c r="I12">
         <v>0</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" t="s" s="0">
+      <c r="A13" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="1">
         <v>45234</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s" s="0">
+      <c r="D13" t="s">
         <v>2</v>
       </c>
-      <c r="E13" t="s" s="0">
+      <c r="E13" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="0">
+      <c r="F13">
         <v>72</v>
       </c>
-      <c r="G13" s="0">
+      <c r="G13">
         <v>44</v>
       </c>
-      <c r="H13" s="0">
+      <c r="H13">
         <v>28</v>
       </c>
-      <c r="I13" s="0">
+      <c r="I13">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" t="s" s="0">
+      <c r="A14" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="1">
         <v>45234</v>
       </c>
-      <c r="C14" t="s" s="0">
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="E14" t="s" s="0">
+      <c r="E14" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="0">
+      <c r="F14">
         <v>97</v>
       </c>
-      <c r="G14" s="0">
+      <c r="G14">
         <v>51</v>
       </c>
-      <c r="H14" s="0">
+      <c r="H14">
         <v>30</v>
       </c>
-      <c r="I14" s="0">
+      <c r="I14">
         <v>0</v>
       </c>
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" t="s" s="0">
+      <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="1">
         <v>45234</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="C15" t="s">
         <v>11</v>
       </c>
-      <c r="D15" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s" s="0">
+      <c r="D15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="0">
+      <c r="F15">
         <v>54</v>
       </c>
-      <c r="G15" s="0">
+      <c r="G15">
         <v>26</v>
       </c>
-      <c r="H15" s="0">
+      <c r="H15">
         <v>28</v>
       </c>
-      <c r="I15" s="0">
+      <c r="I15">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" t="s" s="0">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="1">
         <v>45234</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="D16" t="s" s="0">
+      <c r="D16" t="s">
         <v>2</v>
       </c>
-      <c r="E16" t="s" s="0">
+      <c r="E16" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="0">
+      <c r="F16">
         <v>82</v>
       </c>
-      <c r="G16" s="0">
+      <c r="G16">
         <v>32</v>
       </c>
-      <c r="H16" s="0">
+      <c r="H16">
         <v>50</v>
       </c>
-      <c r="I16" s="0">
+      <c r="I16">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A17" t="s" s="0">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="1">
         <v>45234</v>
       </c>
-      <c r="C17" t="s" s="0">
+      <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s" s="0">
+      <c r="D17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" t="s" s="0">
+      <c r="E17" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="0">
+      <c r="F17">
         <v>60</v>
       </c>
-      <c r="G17" s="0">
+      <c r="G17">
         <v>40</v>
       </c>
-      <c r="H17" s="0">
+      <c r="H17">
         <v>20</v>
       </c>
-      <c r="I17" s="0">
+      <c r="I17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A18" t="s" s="0">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>45234</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" t="s" s="0">
+      <c r="D18" t="s">
         <v>9</v>
       </c>
-      <c r="E18" t="s" s="0">
+      <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="0">
+      <c r="F18">
         <v>56</v>
       </c>
-      <c r="G18" s="0">
+      <c r="G18">
         <v>48</v>
       </c>
-      <c r="H18" s="0">
+      <c r="H18">
         <v>8</v>
       </c>
-      <c r="I18" s="0">
+      <c r="I18">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A19" t="s" s="0">
+      <c r="A19" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="1">
         <v>45234</v>
       </c>
-      <c r="C19" t="s" s="0">
+      <c r="C19" t="s">
         <v>11</v>
       </c>
-      <c r="D19" t="s" s="0">
+      <c r="D19" t="s">
         <v>9</v>
       </c>
-      <c r="E19" t="s" s="0">
+      <c r="E19" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="0">
+      <c r="F19">
         <v>60</v>
       </c>
-      <c r="G19" s="0">
+      <c r="G19">
         <v>30</v>
       </c>
-      <c r="H19" s="0">
+      <c r="H19">
         <v>30</v>
       </c>
-      <c r="I19" s="0">
+      <c r="I19">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A20" t="s" s="0">
+      <c r="A20" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="1">
         <v>45234</v>
       </c>
-      <c r="C20" t="s" s="0">
+      <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" t="s" s="0">
+      <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" t="s" s="0">
+      <c r="E20" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="0">
+      <c r="F20">
         <v>39</v>
       </c>
-      <c r="G20" s="0">
+      <c r="G20">
         <v>34</v>
       </c>
-      <c r="H20" s="0">
+      <c r="H20">
         <v>5</v>
       </c>
-      <c r="I20" s="0">
+      <c r="I20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A21" t="s" s="0">
+      <c r="A21" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="1">
         <v>45241</v>
       </c>
-      <c r="C21" t="s" s="0">
+      <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="D21" t="s" s="0">
+      <c r="D21" t="s">
         <v>9</v>
       </c>
-      <c r="E21" t="s" s="0">
+      <c r="E21" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="0">
+      <c r="F21">
         <v>32</v>
       </c>
-      <c r="G21" s="0">
+      <c r="G21">
         <v>4</v>
       </c>
-      <c r="H21" s="0">
+      <c r="H21">
         <v>28</v>
       </c>
-      <c r="I21" s="0">
-        <v>0</v>
-      </c>
-      <c r="K21" t="s" s="0">
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="K21" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A22" t="s" s="0">
+      <c r="A22" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="1">
         <v>45241</v>
       </c>
-      <c r="C22" t="s" s="0">
+      <c r="C22" t="s">
         <v>4</v>
       </c>
-      <c r="D22" t="s" s="0">
+      <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="E22" t="s" s="0">
+      <c r="E22" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="0">
+      <c r="F22">
         <v>83</v>
       </c>
-      <c r="G22" s="0">
+      <c r="G22">
         <v>55</v>
       </c>
-      <c r="H22" s="0">
+      <c r="H22">
         <v>28</v>
       </c>
-      <c r="I22" s="0">
-        <v>0</v>
-      </c>
-      <c r="K22" t="s" s="0">
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A23" t="s" s="0">
+      <c r="A23" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="1">
         <v>45241</v>
       </c>
-      <c r="C23" t="s" s="0">
+      <c r="C23" t="s">
         <v>3</v>
       </c>
-      <c r="D23" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E23" t="s" s="0">
+      <c r="D23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="0">
+      <c r="F23">
         <v>56</v>
       </c>
-      <c r="G23" s="0">
+      <c r="G23">
         <v>26</v>
       </c>
-      <c r="H23" s="0">
+      <c r="H23">
         <v>30</v>
       </c>
-      <c r="I23" s="0">
-        <v>0</v>
-      </c>
-      <c r="K23" t="s" s="0">
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A24" t="s" s="0">
+      <c r="A24" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="1">
         <v>45241</v>
       </c>
-      <c r="C24" t="s" s="0">
+      <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="D24" t="s" s="0">
+      <c r="D24" t="s">
         <v>9</v>
       </c>
-      <c r="E24" t="s" s="0">
+      <c r="E24" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="0">
+      <c r="F24">
         <v>33</v>
       </c>
-      <c r="G24" s="0">
+      <c r="G24">
         <v>28</v>
       </c>
-      <c r="H24" s="0">
+      <c r="H24">
         <v>5</v>
       </c>
-      <c r="I24" s="0">
-        <v>0</v>
-      </c>
-      <c r="K24" t="s" s="0">
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="K24" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A25" t="s" s="0">
+      <c r="A25" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="1">
         <v>45241</v>
       </c>
-      <c r="C25" t="s" s="0">
+      <c r="C25" t="s">
         <v>4</v>
       </c>
-      <c r="D25" t="s" s="0">
+      <c r="D25" t="s">
         <v>9</v>
       </c>
-      <c r="E25" t="s" s="0">
+      <c r="E25" t="s">
         <v>1</v>
       </c>
-      <c r="F25" s="0">
+      <c r="F25">
         <v>56</v>
       </c>
-      <c r="G25" s="0">
+      <c r="G25">
         <v>36</v>
       </c>
-      <c r="H25" s="0">
+      <c r="H25">
         <v>20</v>
       </c>
-      <c r="I25" s="0">
-        <v>0</v>
-      </c>
-      <c r="K25" t="s" s="0">
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A26" t="s" s="0">
+      <c r="A26" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="1">
         <v>45241</v>
       </c>
-      <c r="C26" t="s" s="0">
+      <c r="C26" t="s">
         <v>3</v>
       </c>
-      <c r="D26" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s" s="0">
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
         <v>1</v>
       </c>
-      <c r="F26" s="0">
+      <c r="F26">
         <v>55</v>
       </c>
-      <c r="G26" s="0">
+      <c r="G26">
         <v>27</v>
       </c>
-      <c r="H26" s="0">
+      <c r="H26">
         <v>28</v>
       </c>
-      <c r="I26" s="0">
-        <v>0</v>
-      </c>
-      <c r="K26" t="s" s="0">
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="K26" t="s">
         <v>50</v>
       </c>
       <c r="T26" s="5"/>
@@ -2409,33 +2408,6 @@
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
     </row>
-    <row r="27">
-      <c r="A27" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="B27" s="0"/>
-      <c r="C27" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="D27" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E27" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="F27" t="n" s="0">
-        <v>20.0</v>
-      </c>
-      <c r="G27" t="n" s="0">
-        <v>20.0</v>
-      </c>
-      <c r="H27" t="n" s="0">
-        <v>20.0</v>
-      </c>
-      <c r="I27" t="n" s="0">
-        <v>10.0</v>
-      </c>
-    </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="T31" s="5"/>
       <c r="U31" s="5"/>
@@ -2443,36 +2415,36 @@
       <c r="W31" s="5"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A32" t="s" s="0">
+      <c r="A32" t="s">
         <v>51</v>
       </c>
-      <c r="F32" s="0">
+      <c r="F32">
         <v>10</v>
       </c>
-      <c r="G32" s="0">
+      <c r="G32">
         <v>10</v>
       </c>
-      <c r="H32" s="0">
+      <c r="H32">
         <v>56</v>
       </c>
-      <c r="I32" s="0">
+      <c r="I32">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" t="s" s="0">
+      <c r="A33" t="s">
         <v>51</v>
       </c>
-      <c r="F33" s="0">
+      <c r="F33">
         <v>10</v>
       </c>
-      <c r="G33" s="0">
+      <c r="G33">
         <v>10</v>
       </c>
-      <c r="H33" s="0">
+      <c r="H33">
         <v>56</v>
       </c>
-      <c r="I33" s="0">
+      <c r="I33">
         <v>0</v>
       </c>
     </row>
@@ -2496,8 +2468,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="10.0"/>
-    <col min="5" max="5" customWidth="true" width="10.6640625"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -2529,7 +2501,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="V2" t="s" s="0">
+      <c r="V2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2537,16 +2509,16 @@
       <c r="A3" s="1">
         <v>45237</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>106</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2554,25 +2526,25 @@
       <c r="A4" s="1">
         <v>45237</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <v>83</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N4" t="s" s="0">
+      <c r="N4" t="s">
         <v>23</v>
       </c>
-      <c r="O4" t="s" s="0">
+      <c r="O4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2580,26 +2552,26 @@
       <c r="A5" s="1">
         <v>45237</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>89</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="M5" t="s" s="0">
+      <c r="M5" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="0">
+      <c r="N5">
         <f>(SUMIF($C$3:$C$100, M5, $B$3:$B$100)/COUNTIF($C$3:$C$100, M5))</f>
         <v>88.083333333333329</v>
       </c>
-      <c r="O5" s="0">
+      <c r="O5">
         <f>(SUMIF($C$3:$C$100, M5, $F$3:$F$100)/COUNTIF($C$13:$C$100, M5))</f>
         <v>42.428571428571431</v>
       </c>
@@ -2608,26 +2580,26 @@
       <c r="A6" s="1">
         <v>45238</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6">
         <v>71</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s" s="0">
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="M6" t="s" s="0">
+      <c r="M6" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="0">
+      <c r="N6">
         <f>(SUMIF($C$3:$C$100, M6, $B$3:$B$100)/COUNTIF($C$3:$C$100, M6))</f>
         <v>98.5</v>
       </c>
-      <c r="O6" s="0">
+      <c r="O6">
         <f>(SUMIF($C$3:$C$100, M6, $F$3:$F$100)/COUNTIF($C$13:$C$100, M6))</f>
         <v>57.333333333333336</v>
       </c>
@@ -2636,26 +2608,26 @@
       <c r="A7" s="1">
         <v>45238</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7">
         <v>88</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s" s="0">
+      <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="M7" t="s" s="0">
+      <c r="M7" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="0">
+      <c r="N7">
         <f>(SUMIF($C$3:$C$100, M7, $B$3:$B$100)/COUNTIF($C$3:$C$100, M7))</f>
         <v>86.25</v>
       </c>
-      <c r="O7" s="0">
+      <c r="O7">
         <f>(SUMIF($C$3:$C$100, M7, $F$3:$F$100)/COUNTIF($C$13:$C$100, M7))</f>
         <v>38</v>
       </c>
@@ -2664,16 +2636,16 @@
       <c r="A8" s="1">
         <v>45238</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8">
         <v>111</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>2</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="E8" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2681,16 +2653,16 @@
       <c r="A9" s="1">
         <v>45238</v>
       </c>
-      <c r="B9" s="0">
+      <c r="B9">
         <v>34</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="D9" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s" s="0">
+      <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="M9" s="2" t="s">
@@ -2701,16 +2673,16 @@
       <c r="A10" s="1">
         <v>45238</v>
       </c>
-      <c r="B10" s="0">
+      <c r="B10">
         <v>120</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s" s="0">
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="H10" s="5" t="s">
@@ -2719,14 +2691,14 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="M10" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="N10" s="0">
+      <c r="M10" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10">
         <f>(SUMIF($D$3:$D$100, M10, $B$3:$B$100)/COUNTIF($D$3:$D$100, M10))</f>
         <v>96.666666666666671</v>
       </c>
-      <c r="O10" s="0">
+      <c r="O10">
         <f>(SUMIF($D$3:$D$100, M10, $F$3:$F$100)/COUNTIF($D$13:$D$100, M10))</f>
         <v>26</v>
       </c>
@@ -2735,16 +2707,16 @@
       <c r="A11" s="1">
         <v>45238</v>
       </c>
-      <c r="B11" s="0">
+      <c r="B11">
         <v>75</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>9</v>
       </c>
-      <c r="E11" t="s" s="0">
+      <c r="E11" t="s">
         <v>1</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -2755,14 +2727,14 @@
         <v>22</v>
       </c>
       <c r="K11" s="5"/>
-      <c r="M11" t="s" s="0">
+      <c r="M11" t="s">
         <v>9</v>
       </c>
-      <c r="N11" s="0">
+      <c r="N11">
         <f>(SUMIF($D$3:$D$100, M11, $B$3:$B$100)/COUNTIF($D$3:$D$100, M11))</f>
         <v>77</v>
       </c>
-      <c r="O11" s="0">
+      <c r="O11">
         <f>(SUMIF($D$3:$D$100, M11, $F$3:$F$100)/COUNTIF($D$13:$D$100, M11))</f>
         <v>45.166666666666664</v>
       </c>
@@ -2780,14 +2752,14 @@
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M12" t="s" s="0">
+      <c r="M12" t="s">
         <v>2</v>
       </c>
-      <c r="N12" s="0">
+      <c r="N12">
         <f>(SUMIF($D$3:$D$100, M12, $B$3:$B$100)/COUNTIF($D$3:$D$100, M12))</f>
         <v>97.75</v>
       </c>
-      <c r="O12" s="0">
+      <c r="O12">
         <f>(SUMIF($D$3:$D$100, M12, $F$3:$F$100)/COUNTIF($D$13:$D$100, M12))</f>
         <v>57.333333333333336</v>
       </c>
@@ -2796,26 +2768,26 @@
       <c r="A13" s="1">
         <v>45237</v>
       </c>
-      <c r="B13" s="0">
+      <c r="B13">
         <v>111</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s" s="0">
+      <c r="D13" t="s">
         <v>2</v>
       </c>
-      <c r="E13" t="s" s="0">
+      <c r="E13" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="0">
+      <c r="F13">
         <v>66</v>
       </c>
-      <c r="H13" s="0">
+      <c r="H13">
         <f t="shared" ref="H13:H23" si="0">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12)+SUMIF($M$15:$M$17, $E13, $N$15:$N$17))/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="I13" s="0">
+      <c r="I13">
         <f t="shared" ref="I13:I23" si="1">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12)+SUMIF($M$15:$M$17, $E13, $O$15:$O$17))/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -2823,7 +2795,7 @@
         <f t="shared" ref="J13:J23" si="2">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12))/2</f>
         <v>98.125</v>
       </c>
-      <c r="K13" s="0">
+      <c r="K13">
         <f t="shared" ref="K13:K23" si="3">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12))/2</f>
         <v>57.333333333333336</v>
       </c>
@@ -2832,26 +2804,26 @@
       <c r="A14" s="1">
         <v>45238</v>
       </c>
-      <c r="B14" s="0">
+      <c r="B14">
         <v>107</v>
       </c>
-      <c r="C14" t="s" s="0">
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="E14" t="s" s="0">
+      <c r="E14" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="0">
+      <c r="F14">
         <v>57</v>
       </c>
-      <c r="H14" s="0">
+      <c r="H14">
         <f t="shared" si="0"/>
         <v>84.49444444444444</v>
       </c>
-      <c r="I14" s="0">
+      <c r="I14">
         <f t="shared" si="1"/>
         <v>48.198412698412703</v>
       </c>
@@ -2859,7 +2831,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K14" s="0">
+      <c r="K14">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -2871,26 +2843,26 @@
       <c r="A15" s="1">
         <v>45234</v>
       </c>
-      <c r="B15" s="0">
+      <c r="B15">
         <v>108</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="C15" t="s">
         <v>3</v>
       </c>
-      <c r="D15" t="s" s="0">
+      <c r="D15" t="s">
         <v>19</v>
       </c>
-      <c r="E15" t="s" s="0">
+      <c r="E15" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="0">
+      <c r="F15">
         <v>38</v>
       </c>
-      <c r="H15" s="0">
+      <c r="H15">
         <f t="shared" si="0"/>
         <v>63.166666666666664</v>
       </c>
-      <c r="I15" s="0">
+      <c r="I15">
         <f t="shared" si="1"/>
         <v>30.166666666666668</v>
       </c>
@@ -2898,18 +2870,18 @@
         <f t="shared" si="2"/>
         <v>43.125</v>
       </c>
-      <c r="K15" s="0">
+      <c r="K15">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="M15" t="s" s="0">
+      <c r="M15" t="s">
         <v>10</v>
       </c>
-      <c r="N15" s="0">
+      <c r="N15">
         <f>(SUMIF($E$3:$E$100, M15, $B$3:$B$100)/COUNTIF($E$3:$E$100, M15))</f>
         <v>83.166666666666671</v>
       </c>
-      <c r="O15" s="0">
+      <c r="O15">
         <f>(SUMIF($E$3:$E$100, M15, $F$3:$F$100)/COUNTIF($E$13:$E$100, M15))</f>
         <v>40</v>
       </c>
@@ -2918,26 +2890,26 @@
       <c r="A16" s="1">
         <v>45234</v>
       </c>
-      <c r="B16" s="0">
+      <c r="B16">
         <v>107</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="D16" t="s" s="0">
+      <c r="D16" t="s">
         <v>2</v>
       </c>
-      <c r="E16" t="s" s="0">
+      <c r="E16" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="0">
+      <c r="F16">
         <v>74</v>
       </c>
-      <c r="H16" s="0">
+      <c r="H16">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I16" s="0">
+      <c r="I16">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -2945,18 +2917,18 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K16" s="0">
+      <c r="K16">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
-      <c r="M16" t="s" s="0">
+      <c r="M16" t="s">
         <v>1</v>
       </c>
-      <c r="N16" s="0">
+      <c r="N16">
         <f>(SUMIF($E$3:$E$100, M16, $B$3:$B$100)/COUNTIF($E$3:$E$100, M16))</f>
         <v>88.4</v>
       </c>
-      <c r="O16" s="0">
+      <c r="O16">
         <f>(SUMIF($E$3:$E$100, M16, $F$3:$F$100)/COUNTIF($E$13:$E$100, M16))</f>
         <v>57</v>
       </c>
@@ -2965,26 +2937,26 @@
       <c r="A17" s="1">
         <v>45234</v>
       </c>
-      <c r="B17" s="0">
+      <c r="B17">
         <v>97</v>
       </c>
-      <c r="C17" t="s" s="0">
+      <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s" s="0">
+      <c r="D17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" t="s" s="0">
+      <c r="E17" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="0">
+      <c r="F17">
         <v>62</v>
       </c>
-      <c r="H17" s="0">
+      <c r="H17">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I17" s="0">
+      <c r="I17">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -2992,18 +2964,18 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K17" s="0">
+      <c r="K17">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
-      <c r="M17" t="s" s="0">
+      <c r="M17" t="s">
         <v>5</v>
       </c>
-      <c r="N17" s="0">
+      <c r="N17">
         <f>(SUMIF($E$3:$E$100, M17, $B$3:$B$100)/COUNTIF($E$3:$E$100, M17))</f>
         <v>103.25</v>
       </c>
-      <c r="O17" s="0">
+      <c r="O17">
         <f>(SUMIF($E$3:$E$100, M17, $F$3:$F$100)/COUNTIF($E$13:$E$100, M17))</f>
         <v>52.5</v>
       </c>
@@ -3012,26 +2984,26 @@
       <c r="A18" s="1">
         <v>45234</v>
       </c>
-      <c r="B18" s="0">
+      <c r="B18">
         <v>99</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s" s="0">
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="0">
+      <c r="F18">
         <v>26</v>
       </c>
-      <c r="H18" s="0">
+      <c r="H18">
         <f t="shared" si="0"/>
         <v>89.305555555555557</v>
       </c>
-      <c r="I18" s="0">
+      <c r="I18">
         <f t="shared" si="1"/>
         <v>36.142857142857146</v>
       </c>
@@ -3039,7 +3011,7 @@
         <f t="shared" si="2"/>
         <v>92.375</v>
       </c>
-      <c r="K18" s="0">
+      <c r="K18">
         <f t="shared" si="3"/>
         <v>34.214285714285715</v>
       </c>
@@ -3048,26 +3020,26 @@
       <c r="A19" s="1">
         <v>45234</v>
       </c>
-      <c r="B19" s="0">
+      <c r="B19">
         <v>87</v>
       </c>
-      <c r="C19" t="s" s="0">
+      <c r="C19" t="s">
         <v>4</v>
       </c>
-      <c r="D19" t="s" s="0">
+      <c r="D19" t="s">
         <v>2</v>
       </c>
-      <c r="E19" t="s" s="0">
+      <c r="E19" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="0">
+      <c r="F19">
         <v>32</v>
       </c>
-      <c r="H19" s="0">
+      <c r="H19">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I19" s="0">
+      <c r="I19">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -3075,7 +3047,7 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K19" s="0">
+      <c r="K19">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
@@ -3084,26 +3056,26 @@
       <c r="A20" s="1">
         <v>45234</v>
       </c>
-      <c r="B20" s="0">
+      <c r="B20">
         <v>76</v>
       </c>
-      <c r="C20" t="s" s="0">
+      <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" t="s" s="0">
+      <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" t="s" s="0">
+      <c r="E20" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="0">
+      <c r="F20">
         <v>48</v>
       </c>
-      <c r="H20" s="0">
+      <c r="H20">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I20" s="0">
+      <c r="I20">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3111,7 +3083,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K20" s="0">
+      <c r="K20">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3120,26 +3092,26 @@
       <c r="A21" s="1">
         <v>45234</v>
       </c>
-      <c r="B21" s="0">
+      <c r="B21">
         <v>93</v>
       </c>
-      <c r="C21" t="s" s="0">
+      <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="D21" t="s" s="0">
+      <c r="D21" t="s">
         <v>9</v>
       </c>
-      <c r="E21" t="s" s="0">
+      <c r="E21" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="0">
+      <c r="F21">
         <v>40</v>
       </c>
-      <c r="H21" s="0">
+      <c r="H21">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I21" s="0">
+      <c r="I21">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3147,7 +3119,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K21" s="0">
+      <c r="K21">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3156,26 +3128,26 @@
       <c r="A22" s="1">
         <v>45234</v>
       </c>
-      <c r="B22" s="0">
+      <c r="B22">
         <v>85</v>
       </c>
-      <c r="C22" t="s" s="0">
+      <c r="C22" t="s">
         <v>11</v>
       </c>
-      <c r="D22" t="s" s="0">
+      <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="E22" t="s" s="0">
+      <c r="E22" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="0">
+      <c r="F22">
         <v>30</v>
       </c>
-      <c r="H22" s="0">
+      <c r="H22">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I22" s="0">
+      <c r="I22">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3183,7 +3155,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K22" s="0">
+      <c r="K22">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3192,26 +3164,26 @@
       <c r="A23" s="1">
         <v>45234</v>
       </c>
-      <c r="B23" s="0">
+      <c r="B23">
         <v>49</v>
       </c>
-      <c r="C23" t="s" s="0">
+      <c r="C23" t="s">
         <v>11</v>
       </c>
-      <c r="D23" t="s" s="0">
+      <c r="D23" t="s">
         <v>9</v>
       </c>
-      <c r="E23" t="s" s="0">
+      <c r="E23" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="0">
+      <c r="F23">
         <v>34</v>
       </c>
-      <c r="H23" s="0">
+      <c r="H23">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I23" s="0">
+      <c r="I23">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3219,7 +3191,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K23" s="0">
+      <c r="K23">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3239,67 +3211,67 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T28" s="0">
+      <c r="T28">
         <v>1</v>
       </c>
-      <c r="U28" t="s" s="0">
+      <c r="U28" t="s">
         <v>3</v>
       </c>
-      <c r="V28" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="W28" t="s" s="0">
+      <c r="V28" t="s">
+        <v>0</v>
+      </c>
+      <c r="W28" t="s">
         <v>1</v>
       </c>
-      <c r="X28" s="0">
+      <c r="X28">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y28" s="0">
+      <c r="Y28">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T29" s="0">
+      <c r="T29">
         <v>2</v>
       </c>
-      <c r="U29" t="s" s="0">
+      <c r="U29" t="s">
         <v>11</v>
       </c>
-      <c r="V29" t="s" s="0">
+      <c r="V29" t="s">
         <v>9</v>
       </c>
-      <c r="W29" t="s" s="0">
+      <c r="W29" t="s">
         <v>1</v>
       </c>
-      <c r="X29" s="0">
+      <c r="X29">
         <f>(N5+N11+N16)/3</f>
         <v>84.49444444444444</v>
       </c>
-      <c r="Y29" s="0">
+      <c r="Y29">
         <f>(O5+O11+O16)/3</f>
         <v>48.198412698412703</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T30" s="0">
+      <c r="T30">
         <v>3</v>
       </c>
-      <c r="U30" t="s" s="0">
+      <c r="U30" t="s">
         <v>4</v>
       </c>
-      <c r="V30" t="s" s="0">
+      <c r="V30" t="s">
         <v>9</v>
       </c>
-      <c r="W30" t="s" s="0">
+      <c r="W30" t="s">
         <v>1</v>
       </c>
-      <c r="X30" s="0">
+      <c r="X30">
         <f>(N6+N11+N16)/3</f>
         <v>87.966666666666654</v>
       </c>
-      <c r="Y30" s="0">
+      <c r="Y30">
         <f>(O6+O11+O16)/3</f>
         <v>53.166666666666664</v>
       </c>
@@ -3313,67 +3285,67 @@
       <c r="W32" s="5"/>
     </row>
     <row r="33" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T33" s="0">
+      <c r="T33">
         <v>1</v>
       </c>
-      <c r="U33" t="s" s="0">
+      <c r="U33" t="s">
         <v>3</v>
       </c>
-      <c r="V33" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="W33" t="s" s="0">
+      <c r="V33" t="s">
+        <v>0</v>
+      </c>
+      <c r="W33" t="s">
         <v>1</v>
       </c>
-      <c r="X33" s="0">
+      <c r="X33">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y33" s="0">
+      <c r="Y33">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="34" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T34" s="0">
+      <c r="T34">
         <v>2</v>
       </c>
-      <c r="U34" t="s" s="0">
+      <c r="U34" t="s">
         <v>11</v>
       </c>
-      <c r="V34" t="s" s="0">
+      <c r="V34" t="s">
         <v>9</v>
       </c>
-      <c r="W34" t="s" s="0">
+      <c r="W34" t="s">
         <v>10</v>
       </c>
-      <c r="X34" s="0">
+      <c r="X34">
         <f>(N5+N11+N15)/3</f>
         <v>82.75</v>
       </c>
-      <c r="Y34" s="0">
+      <c r="Y34">
         <f>(O5+O11+O15)/3</f>
         <v>42.531746031746032</v>
       </c>
     </row>
     <row r="35" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T35" s="0">
+      <c r="T35">
         <v>3</v>
       </c>
-      <c r="U35" t="s" s="0">
+      <c r="U35" t="s">
         <v>4</v>
       </c>
-      <c r="V35" t="s" s="0">
+      <c r="V35" t="s">
         <v>2</v>
       </c>
-      <c r="W35" t="s" s="0">
+      <c r="W35" t="s">
         <v>5</v>
       </c>
-      <c r="X35" s="0">
+      <c r="X35">
         <f>(N6+N12+N17)/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="Y35" s="0">
+      <c r="Y35">
         <f>(O6+O12+O17)/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -3403,289 +3375,289 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="H1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>70.642857142857139</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <v>35.333333333333336</v>
       </c>
-      <c r="C2" s="0">
+      <c r="C2">
         <v>22.666666666666668</v>
       </c>
-      <c r="D2" s="0">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
         <v>70.563855421704886</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2">
         <v>34.628352490586749</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2">
         <v>22.754789272009987</v>
       </c>
-      <c r="H2" s="0">
-        <v>0</v>
-      </c>
-      <c r="M2" t="s" s="0">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>82.166666666666671</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>46.6</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3">
         <v>34.200000000000003</v>
       </c>
-      <c r="D3" s="0">
-        <v>0</v>
-      </c>
-      <c r="E3" s="0">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <v>81.78021978030641</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3">
         <v>46.881578947305435</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G3">
         <v>33.473684210688774</v>
       </c>
-      <c r="H3" s="0">
-        <v>0</v>
-      </c>
-      <c r="M3" t="s" s="0">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>73.25</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <v>26</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4">
         <v>30</v>
       </c>
-      <c r="D4" s="0">
-        <v>0</v>
-      </c>
-      <c r="E4" s="0">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>72.761904762010133</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F4">
         <v>26</v>
       </c>
-      <c r="G4" s="0">
+      <c r="G4">
         <v>30</v>
       </c>
-      <c r="H4" s="0">
-        <v>0</v>
-      </c>
-      <c r="M4" t="s" s="0">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>61</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>38.299999999999997</v>
       </c>
-      <c r="C5" s="0">
+      <c r="C5">
         <v>22.4</v>
       </c>
-      <c r="D5" s="0">
-        <v>0</v>
-      </c>
-      <c r="E5" s="0">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
         <v>60.593406593497761</v>
       </c>
-      <c r="F5" s="0">
+      <c r="F5">
         <v>37.847682119307144</v>
       </c>
-      <c r="G5" s="0">
+      <c r="G5">
         <v>22.566225165525484</v>
       </c>
-      <c r="H5" s="0">
-        <v>0</v>
-      </c>
-      <c r="M5" t="s" s="0">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>92.75</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6">
         <v>47.333333333333336</v>
       </c>
-      <c r="C6" s="0">
+      <c r="C6">
         <v>41</v>
       </c>
-      <c r="D6" s="0">
-        <v>0</v>
-      </c>
-      <c r="E6" s="0">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>93.207627118538568</v>
       </c>
-      <c r="F6" s="0">
+      <c r="F6">
         <v>47.999999999838096</v>
       </c>
-      <c r="G6" s="0">
+      <c r="G6">
         <v>41.142857142822443</v>
       </c>
-      <c r="H6" s="0">
-        <v>0</v>
-      </c>
-      <c r="M6" t="s" s="0">
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>75.25</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7">
         <v>26</v>
       </c>
-      <c r="C7" s="0">
+      <c r="C7">
         <v>29</v>
       </c>
-      <c r="D7" s="0">
-        <v>0</v>
-      </c>
-      <c r="E7" s="0">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
         <v>75.471544715398167</v>
       </c>
-      <c r="F7" s="0">
+      <c r="F7">
         <v>25.999999999999996</v>
       </c>
-      <c r="G7" s="0">
+      <c r="G7">
         <v>29.114754098335069</v>
       </c>
-      <c r="H7" s="0">
-        <v>0</v>
-      </c>
-      <c r="M7" t="s" s="0">
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="0">
+      <c r="A8">
         <v>61</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8">
         <v>38.166666666666664</v>
       </c>
-      <c r="C8" s="0">
+      <c r="C8">
         <v>20.166666666666668</v>
       </c>
-      <c r="D8" s="0">
-        <v>0</v>
-      </c>
-      <c r="E8" s="0">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
         <v>60.999999999999986</v>
       </c>
-      <c r="F8" s="0">
+      <c r="F8">
         <v>38.166666666666664</v>
       </c>
-      <c r="G8" s="0">
+      <c r="G8">
         <v>20.166666666666664</v>
       </c>
-      <c r="H8" s="0">
-        <v>0</v>
-      </c>
-      <c r="M8" t="s" s="0">
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="0">
+      <c r="A9">
         <v>88.333333333333329</v>
       </c>
-      <c r="B9" s="0">
+      <c r="B9">
         <v>47.333333333333336</v>
       </c>
-      <c r="C9" s="0">
+      <c r="C9">
         <v>41</v>
       </c>
-      <c r="D9" s="0">
-        <v>0</v>
-      </c>
-      <c r="E9" s="0">
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
         <v>89.142857142660532</v>
       </c>
-      <c r="F9" s="0">
+      <c r="F9">
         <v>47.999999999838096</v>
       </c>
-      <c r="G9" s="0">
+      <c r="G9">
         <v>41.142857142822443</v>
       </c>
-      <c r="H9" s="0">
-        <v>0</v>
-      </c>
-      <c r="M9" t="s" s="0">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="0">
+      <c r="A10">
         <v>76.266666666666666</v>
       </c>
-      <c r="B10" s="0">
+      <c r="B10">
         <v>34.333333333333336</v>
       </c>
-      <c r="C10" s="0">
+      <c r="C10">
         <v>26.833333333333332</v>
       </c>
-      <c r="D10" s="0">
-        <v>0</v>
-      </c>
-      <c r="E10" s="0">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
         <v>75.400419287396943</v>
       </c>
-      <c r="F10" s="0">
+      <c r="F10">
         <v>33.995024875690561</v>
       </c>
-      <c r="G10" s="0">
+      <c r="G10">
         <v>26.487562189124915</v>
       </c>
-      <c r="H10" s="0">
-        <v>0</v>
-      </c>
-      <c r="M10" t="s" s="0">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="M10" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor changes, i'm done for today
</commit_message>
<xml_diff>
--- a/Drive Teams.xlsx
+++ b/Drive Teams.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -200,6 +200,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1667,8 +1668,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="10.0"/>
+    <col min="5" max="5" customWidth="true" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -1701,25 +1702,25 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B2" s="1">
         <v>45237</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>106</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="0">
         <v>0</v>
       </c>
       <c r="M2" s="2"/>
@@ -1732,673 +1733,673 @@
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B3" s="1">
         <v>45237</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>83</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B4" s="1">
         <v>45237</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>89</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="0">
         <v>0</v>
       </c>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>45238</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>71</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B6" s="1">
         <v>45238</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>88</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B7" s="1">
         <v>45238</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0">
         <v>111</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B8" s="1">
         <v>45238</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0">
         <v>34</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>45238</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D9" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="0">
         <v>120</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="0">
         <v>0</v>
       </c>
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B10" s="1">
         <v>45238</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="0">
         <v>75</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>45237</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="0">
         <v>111</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="0">
         <v>66</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="0">
         <v>45</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>45238</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="0">
         <v>107</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="0">
         <v>57</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="0">
         <v>50</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="0">
         <v>0</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B13" s="1">
         <v>45234</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="0">
         <v>72</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="0">
         <v>44</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="0">
         <v>28</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B14" s="1">
         <v>45234</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="0">
         <v>97</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="0">
         <v>51</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="0">
         <v>30</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="0">
         <v>0</v>
       </c>
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B15" s="1">
         <v>45234</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="D15" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="0">
         <v>54</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="0">
         <v>26</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="0">
         <v>28</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B16" s="1">
         <v>45234</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="0">
         <v>82</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="0">
         <v>32</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="0">
         <v>50</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B17" s="1">
         <v>45234</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="0">
         <v>60</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="0">
         <v>40</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="0">
         <v>20</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>45234</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="0">
         <v>56</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="0">
         <v>48</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="0">
         <v>8</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B19" s="1">
         <v>45234</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="0">
         <v>60</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="0">
         <v>30</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="0">
         <v>30</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B20" s="1">
         <v>45234</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="0">
         <v>39</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="0">
         <v>34</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="0">
         <v>5</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B21" s="1">
         <v>45241</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="0">
         <v>32</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="0">
         <v>4</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="0">
         <v>28</v>
       </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="K21" t="s">
+      <c r="I21" s="0">
+        <v>0</v>
+      </c>
+      <c r="K21" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B22" s="1">
         <v>45241</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="0">
         <v>83</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="0">
         <v>55</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="0">
         <v>28</v>
       </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="K22" t="s">
+      <c r="I22" s="0">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B23" s="1">
         <v>45241</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D23" t="s">
-        <v>0</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="D23" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="0">
         <v>56</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="0">
         <v>26</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="0">
         <v>30</v>
       </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="I23" s="0">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B24" s="1">
         <v>45241</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="0">
         <v>33</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="0">
         <v>28</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="0">
         <v>5</v>
       </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="K24" t="s">
+      <c r="I24" s="0">
+        <v>0</v>
+      </c>
+      <c r="K24" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B25" s="1">
         <v>45241</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="0">
         <v>56</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="0">
         <v>36</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="0">
         <v>20</v>
       </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="K25" t="s">
+      <c r="I25" s="0">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B26" s="1">
         <v>45241</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="D26" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="0">
         <v>55</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="0">
         <v>27</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="0">
         <v>28</v>
       </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="K26" t="s">
+      <c r="I26" s="0">
+        <v>0</v>
+      </c>
+      <c r="K26" t="s" s="0">
         <v>50</v>
       </c>
       <c r="T26" s="5"/>
@@ -2415,36 +2416,36 @@
       <c r="W31" s="5"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="0">
         <v>10</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="0">
         <v>10</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="0">
         <v>56</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="0">
         <v>10</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="0">
         <v>10</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="0">
         <v>56</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2468,8 +2469,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="10.0"/>
+    <col min="5" max="5" customWidth="true" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -2501,7 +2502,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="V2" t="s">
+      <c r="V2" t="s" s="0">
         <v>18</v>
       </c>
     </row>
@@ -2509,16 +2510,16 @@
       <c r="A3" s="1">
         <v>45237</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <v>106</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>1</v>
       </c>
     </row>
@@ -2526,25 +2527,25 @@
       <c r="A4" s="1">
         <v>45237</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0">
         <v>83</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" t="s" s="0">
         <v>24</v>
       </c>
     </row>
@@ -2552,26 +2553,26 @@
       <c r="A5" s="1">
         <v>45237</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0">
         <v>89</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="0">
         <f>(SUMIF($C$3:$C$100, M5, $B$3:$B$100)/COUNTIF($C$3:$C$100, M5))</f>
         <v>88.083333333333329</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="0">
         <f>(SUMIF($C$3:$C$100, M5, $F$3:$F$100)/COUNTIF($C$13:$C$100, M5))</f>
         <v>42.428571428571431</v>
       </c>
@@ -2580,26 +2581,26 @@
       <c r="A6" s="1">
         <v>45238</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="0">
         <v>71</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="0">
         <f>(SUMIF($C$3:$C$100, M6, $B$3:$B$100)/COUNTIF($C$3:$C$100, M6))</f>
         <v>98.5</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="0">
         <f>(SUMIF($C$3:$C$100, M6, $F$3:$F$100)/COUNTIF($C$13:$C$100, M6))</f>
         <v>57.333333333333336</v>
       </c>
@@ -2608,26 +2609,26 @@
       <c r="A7" s="1">
         <v>45238</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="0">
         <v>88</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="0">
         <f>(SUMIF($C$3:$C$100, M7, $B$3:$B$100)/COUNTIF($C$3:$C$100, M7))</f>
         <v>86.25</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="0">
         <f>(SUMIF($C$3:$C$100, M7, $F$3:$F$100)/COUNTIF($C$13:$C$100, M7))</f>
         <v>38</v>
       </c>
@@ -2636,16 +2637,16 @@
       <c r="A8" s="1">
         <v>45238</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="0">
         <v>111</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>1</v>
       </c>
     </row>
@@ -2653,16 +2654,16 @@
       <c r="A9" s="1">
         <v>45238</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="0">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>1</v>
       </c>
       <c r="M9" s="2" t="s">
@@ -2673,16 +2674,16 @@
       <c r="A10" s="1">
         <v>45238</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="0">
         <v>120</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D10" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s" s="0">
         <v>1</v>
       </c>
       <c r="H10" s="5" t="s">
@@ -2691,14 +2692,14 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="M10" t="s">
-        <v>0</v>
-      </c>
-      <c r="N10">
+      <c r="M10" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="N10" s="0">
         <f>(SUMIF($D$3:$D$100, M10, $B$3:$B$100)/COUNTIF($D$3:$D$100, M10))</f>
         <v>96.666666666666671</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="0">
         <f>(SUMIF($D$3:$D$100, M10, $F$3:$F$100)/COUNTIF($D$13:$D$100, M10))</f>
         <v>26</v>
       </c>
@@ -2707,16 +2708,16 @@
       <c r="A11" s="1">
         <v>45238</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="0">
         <v>75</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>1</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -2727,14 +2728,14 @@
         <v>22</v>
       </c>
       <c r="K11" s="5"/>
-      <c r="M11" t="s">
+      <c r="M11" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="0">
         <f>(SUMIF($D$3:$D$100, M11, $B$3:$B$100)/COUNTIF($D$3:$D$100, M11))</f>
         <v>77</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="0">
         <f>(SUMIF($D$3:$D$100, M11, $F$3:$F$100)/COUNTIF($D$13:$D$100, M11))</f>
         <v>45.166666666666664</v>
       </c>
@@ -2752,14 +2753,14 @@
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="0">
         <f>(SUMIF($D$3:$D$100, M12, $B$3:$B$100)/COUNTIF($D$3:$D$100, M12))</f>
         <v>97.75</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="0">
         <f>(SUMIF($D$3:$D$100, M12, $F$3:$F$100)/COUNTIF($D$13:$D$100, M12))</f>
         <v>57.333333333333336</v>
       </c>
@@ -2768,26 +2769,26 @@
       <c r="A13" s="1">
         <v>45237</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="0">
         <v>111</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="0">
         <v>66</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="0">
         <f t="shared" ref="H13:H23" si="0">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12)+SUMIF($M$15:$M$17, $E13, $N$15:$N$17))/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="0">
         <f t="shared" ref="I13:I23" si="1">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12)+SUMIF($M$15:$M$17, $E13, $O$15:$O$17))/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -2795,7 +2796,7 @@
         <f t="shared" ref="J13:J23" si="2">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12))/2</f>
         <v>98.125</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="0">
         <f t="shared" ref="K13:K23" si="3">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12))/2</f>
         <v>57.333333333333336</v>
       </c>
@@ -2804,26 +2805,26 @@
       <c r="A14" s="1">
         <v>45238</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="0">
         <v>107</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="0">
         <v>57</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="0">
         <f t="shared" si="0"/>
         <v>84.49444444444444</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="0">
         <f t="shared" si="1"/>
         <v>48.198412698412703</v>
       </c>
@@ -2831,7 +2832,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -2843,26 +2844,26 @@
       <c r="A15" s="1">
         <v>45234</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="0">
         <v>108</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="0">
         <v>38</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="0">
         <f t="shared" si="0"/>
         <v>63.166666666666664</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="0">
         <f t="shared" si="1"/>
         <v>30.166666666666668</v>
       </c>
@@ -2870,18 +2871,18 @@
         <f t="shared" si="2"/>
         <v>43.125</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="0">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M15" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="0">
         <f>(SUMIF($E$3:$E$100, M15, $B$3:$B$100)/COUNTIF($E$3:$E$100, M15))</f>
         <v>83.166666666666671</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="0">
         <f>(SUMIF($E$3:$E$100, M15, $F$3:$F$100)/COUNTIF($E$13:$E$100, M15))</f>
         <v>40</v>
       </c>
@@ -2890,26 +2891,26 @@
       <c r="A16" s="1">
         <v>45234</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="0">
         <v>107</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="0">
         <v>74</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="0">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="0">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -2917,18 +2918,18 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="0">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="0">
         <f>(SUMIF($E$3:$E$100, M16, $B$3:$B$100)/COUNTIF($E$3:$E$100, M16))</f>
         <v>88.4</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="0">
         <f>(SUMIF($E$3:$E$100, M16, $F$3:$F$100)/COUNTIF($E$13:$E$100, M16))</f>
         <v>57</v>
       </c>
@@ -2937,26 +2938,26 @@
       <c r="A17" s="1">
         <v>45234</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="0">
         <v>97</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="0">
         <v>62</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -2964,18 +2965,18 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="0">
         <f>(SUMIF($E$3:$E$100, M17, $B$3:$B$100)/COUNTIF($E$3:$E$100, M17))</f>
         <v>103.25</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="0">
         <f>(SUMIF($E$3:$E$100, M17, $F$3:$F$100)/COUNTIF($E$13:$E$100, M17))</f>
         <v>52.5</v>
       </c>
@@ -2984,26 +2985,26 @@
       <c r="A18" s="1">
         <v>45234</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="0">
         <v>99</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D18" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="0">
         <v>26</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="0">
         <f t="shared" si="0"/>
         <v>89.305555555555557</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="0">
         <f t="shared" si="1"/>
         <v>36.142857142857146</v>
       </c>
@@ -3011,7 +3012,7 @@
         <f t="shared" si="2"/>
         <v>92.375</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="0">
         <f t="shared" si="3"/>
         <v>34.214285714285715</v>
       </c>
@@ -3020,26 +3021,26 @@
       <c r="A19" s="1">
         <v>45234</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="0">
         <v>87</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="0">
         <v>32</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="0">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="0">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -3047,7 +3048,7 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="0">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
@@ -3056,26 +3057,26 @@
       <c r="A20" s="1">
         <v>45234</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="0">
         <v>76</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="0">
         <v>48</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3083,7 +3084,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3092,26 +3093,26 @@
       <c r="A21" s="1">
         <v>45234</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="0">
         <v>93</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="0">
         <v>40</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3119,7 +3120,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3128,26 +3129,26 @@
       <c r="A22" s="1">
         <v>45234</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="0">
         <v>85</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="0">
         <v>30</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3155,7 +3156,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3164,26 +3165,26 @@
       <c r="A23" s="1">
         <v>45234</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="0">
         <v>49</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="0">
         <v>34</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3191,7 +3192,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3211,67 +3212,67 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T28">
+      <c r="T28" s="0">
         <v>1</v>
       </c>
-      <c r="U28" t="s">
+      <c r="U28" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="V28" t="s">
-        <v>0</v>
-      </c>
-      <c r="W28" t="s">
+      <c r="V28" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="W28" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X28">
+      <c r="X28" s="0">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y28">
+      <c r="Y28" s="0">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T29">
+      <c r="T29" s="0">
         <v>2</v>
       </c>
-      <c r="U29" t="s">
+      <c r="U29" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="V29" t="s">
+      <c r="V29" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="W29" t="s">
+      <c r="W29" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X29">
+      <c r="X29" s="0">
         <f>(N5+N11+N16)/3</f>
         <v>84.49444444444444</v>
       </c>
-      <c r="Y29">
+      <c r="Y29" s="0">
         <f>(O5+O11+O16)/3</f>
         <v>48.198412698412703</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T30">
+      <c r="T30" s="0">
         <v>3</v>
       </c>
-      <c r="U30" t="s">
+      <c r="U30" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="V30" t="s">
+      <c r="V30" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="W30" t="s">
+      <c r="W30" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X30">
+      <c r="X30" s="0">
         <f>(N6+N11+N16)/3</f>
         <v>87.966666666666654</v>
       </c>
-      <c r="Y30">
+      <c r="Y30" s="0">
         <f>(O6+O11+O16)/3</f>
         <v>53.166666666666664</v>
       </c>
@@ -3285,67 +3286,67 @@
       <c r="W32" s="5"/>
     </row>
     <row r="33" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T33">
+      <c r="T33" s="0">
         <v>1</v>
       </c>
-      <c r="U33" t="s">
+      <c r="U33" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="V33" t="s">
-        <v>0</v>
-      </c>
-      <c r="W33" t="s">
+      <c r="V33" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="W33" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X33">
+      <c r="X33" s="0">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y33">
+      <c r="Y33" s="0">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="34" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T34">
+      <c r="T34" s="0">
         <v>2</v>
       </c>
-      <c r="U34" t="s">
+      <c r="U34" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="V34" t="s">
+      <c r="V34" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="W34" t="s">
+      <c r="W34" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="X34">
+      <c r="X34" s="0">
         <f>(N5+N11+N15)/3</f>
         <v>82.75</v>
       </c>
-      <c r="Y34">
+      <c r="Y34" s="0">
         <f>(O5+O11+O15)/3</f>
         <v>42.531746031746032</v>
       </c>
     </row>
     <row r="35" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T35">
+      <c r="T35" s="0">
         <v>3</v>
       </c>
-      <c r="U35" t="s">
+      <c r="U35" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="V35" t="s">
+      <c r="V35" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="W35" t="s">
+      <c r="W35" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="X35">
+      <c r="X35" s="0">
         <f>(N6+N12+N17)/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="Y35">
+      <c r="Y35" s="0">
         <f>(O6+O12+O17)/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -3375,289 +3376,289 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>70.642857142857139</v>
-      </c>
-      <c r="B2">
+      <c r="A2" t="n" s="0">
+        <v>70.64285714285714</v>
+      </c>
+      <c r="B2" t="n" s="0">
         <v>35.333333333333336</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n" s="0">
         <v>22.666666666666668</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>70.563855421704886</v>
-      </c>
-      <c r="F2">
-        <v>34.628352490586749</v>
-      </c>
-      <c r="G2">
-        <v>22.754789272009987</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="D2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>70.56109725687725</v>
+      </c>
+      <c r="F2" t="n" s="0">
+        <v>34.60317460335194</v>
+      </c>
+      <c r="G2" t="n" s="0">
+        <v>22.757936507914348</v>
+      </c>
+      <c r="H2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M2" t="s" s="0">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>82.166666666666671</v>
-      </c>
-      <c r="B3">
+      <c r="A3" t="n" s="0">
+        <v>82.16666666666667</v>
+      </c>
+      <c r="B3" t="n" s="0">
         <v>46.6</v>
       </c>
-      <c r="C3">
-        <v>34.200000000000003</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>81.78021978030641</v>
-      </c>
-      <c r="F3">
-        <v>46.881578947305435</v>
-      </c>
-      <c r="G3">
-        <v>33.473684210688774</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="C3" t="n" s="0">
+        <v>34.2</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>81.76704545463811</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>46.8911564625177</v>
+      </c>
+      <c r="G3" t="n" s="0">
+        <v>33.44897959201044</v>
+      </c>
+      <c r="H3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M3" t="s" s="0">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>73.25</v>
-      </c>
-      <c r="B4">
-        <v>26</v>
-      </c>
-      <c r="C4">
-        <v>30</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>72.761904762010133</v>
-      </c>
-      <c r="F4">
-        <v>26</v>
-      </c>
-      <c r="G4">
-        <v>30</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="A4" t="n" s="0">
+        <v>69.6</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>26.5</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>29.0</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>68.96774193562257</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>26.5</v>
+      </c>
+      <c r="G4" t="n" s="0">
+        <v>29.0</v>
+      </c>
+      <c r="H4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M4" t="s" s="0">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>61</v>
-      </c>
-      <c r="B5">
-        <v>38.299999999999997</v>
-      </c>
-      <c r="C5">
+      <c r="A5" t="n" s="0">
+        <v>61.0</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>38.3</v>
+      </c>
+      <c r="C5" t="n" s="0">
         <v>22.4</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>60.593406593497761</v>
-      </c>
-      <c r="F5">
-        <v>37.847682119307144</v>
-      </c>
-      <c r="G5">
-        <v>22.566225165525484</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="D5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E5" t="n" s="0">
+        <v>60.57954545464293</v>
+      </c>
+      <c r="F5" t="n" s="0">
+        <v>37.83219178093086</v>
+      </c>
+      <c r="G5" t="n" s="0">
+        <v>22.571917808179144</v>
+      </c>
+      <c r="H5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M5" t="s" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" t="n" s="0">
         <v>92.75</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n" s="0">
         <v>47.333333333333336</v>
       </c>
-      <c r="C6">
-        <v>41</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>93.207627118538568</v>
-      </c>
-      <c r="F6">
-        <v>47.999999999838096</v>
-      </c>
-      <c r="G6">
-        <v>41.142857142822443</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="C6" t="n" s="0">
+        <v>41.0</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E6" t="n" s="0">
+        <v>93.22368421041327</v>
+      </c>
+      <c r="F6" t="n" s="0">
+        <v>48.024691357850564</v>
+      </c>
+      <c r="G6" t="n" s="0">
+        <v>41.148148148110835</v>
+      </c>
+      <c r="H6" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M6" t="s" s="0">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>75.25</v>
-      </c>
-      <c r="B7">
-        <v>26</v>
-      </c>
-      <c r="C7">
-        <v>29</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>75.471544715398167</v>
-      </c>
-      <c r="F7">
-        <v>25.999999999999996</v>
-      </c>
-      <c r="G7">
-        <v>29.114754098335069</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="A7" t="n" s="0">
+        <v>71.2</v>
+      </c>
+      <c r="B7" t="n" s="0">
+        <v>26.333333333333332</v>
+      </c>
+      <c r="C7" t="n" s="0">
+        <v>28.666666666666668</v>
+      </c>
+      <c r="D7" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E7" t="n" s="0">
+        <v>71.03289473687948</v>
+      </c>
+      <c r="F7" t="n" s="0">
+        <v>26.35869565216829</v>
+      </c>
+      <c r="G7" t="n" s="0">
+        <v>28.71739130433658</v>
+      </c>
+      <c r="H7" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M7" t="s" s="0">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>61</v>
-      </c>
-      <c r="B8">
+      <c r="A8" t="n" s="0">
+        <v>61.0</v>
+      </c>
+      <c r="B8" t="n" s="0">
         <v>38.166666666666664</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="n" s="0">
         <v>20.166666666666668</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>60.999999999999986</v>
-      </c>
-      <c r="F8">
-        <v>38.166666666666664</v>
-      </c>
-      <c r="G8">
+      <c r="D8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E8" t="n" s="0">
+        <v>61.0</v>
+      </c>
+      <c r="F8" t="n" s="0">
+        <v>38.16666666666667</v>
+      </c>
+      <c r="G8" t="n" s="0">
         <v>20.166666666666664</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="H8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M8" t="s" s="0">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>88.333333333333329</v>
-      </c>
-      <c r="B9">
+      <c r="A9" t="n" s="0">
+        <v>88.33333333333333</v>
+      </c>
+      <c r="B9" t="n" s="0">
         <v>47.333333333333336</v>
       </c>
-      <c r="C9">
-        <v>41</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>89.142857142660532</v>
-      </c>
-      <c r="F9">
-        <v>47.999999999838096</v>
-      </c>
-      <c r="G9">
-        <v>41.142857142822443</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="C9" t="n" s="0">
+        <v>41.0</v>
+      </c>
+      <c r="D9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E9" t="n" s="0">
+        <v>89.1728395059614</v>
+      </c>
+      <c r="F9" t="n" s="0">
+        <v>48.024691357850564</v>
+      </c>
+      <c r="G9" t="n" s="0">
+        <v>41.148148148110835</v>
+      </c>
+      <c r="H9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M9" t="s" s="0">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>76.266666666666666</v>
-      </c>
-      <c r="B10">
-        <v>34.333333333333336</v>
-      </c>
-      <c r="C10">
-        <v>26.833333333333332</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>75.400419287396943</v>
-      </c>
-      <c r="F10">
-        <v>33.995024875690561</v>
-      </c>
-      <c r="G10">
-        <v>26.487562189124915</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="M10" t="s">
+      <c r="A10" t="n" s="0">
+        <v>74.9375</v>
+      </c>
+      <c r="B10" t="n" s="0">
+        <v>33.285714285714285</v>
+      </c>
+      <c r="C10" t="n" s="0">
+        <v>27.0</v>
+      </c>
+      <c r="D10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E10" t="n" s="0">
+        <v>74.01414141434437</v>
+      </c>
+      <c r="F10" t="n" s="0">
+        <v>32.973684210591465</v>
+      </c>
+      <c r="G10" t="n" s="0">
+        <v>26.69736842111582</v>
+      </c>
+      <c r="H10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M10" t="s" s="0">
         <v>49</v>
       </c>
     </row>

</xml_diff>